<commit_message>
Scripting DPLKKPS001-020 until DPLKKPS001-023
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS001-022 - Kepesertaan - Setup Jenis Alamat Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKPS001-022 - Kepesertaan - Setup Jenis Alamat Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55443B49-B93B-4A11-9F29-23FC22F0C321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5912CCDD-13D1-4478-AD07-A67B10D1AF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>